<commit_message>
added g, validation needed
</commit_message>
<xml_diff>
--- a/Thesis/Resources/initialPerformance.xlsx
+++ b/Thesis/Resources/initialPerformance.xlsx
@@ -43,13 +43,13 @@
     <t xml:space="preserve">Seconds</t>
   </si>
   <si>
-    <t xml:space="preserve">Overall_128_16</t>
+    <t xml:space="preserve">Overall_128</t>
   </si>
   <si>
     <t xml:space="preserve">Overall_128_8</t>
   </si>
   <si>
-    <t xml:space="preserve">Iteration_128_16</t>
+    <t xml:space="preserve">Iteration_128</t>
   </si>
   <si>
     <t xml:space="preserve">Iteration_128_8</t>
@@ -91,13 +91,13 @@
     <t xml:space="preserve">Cavity_256_8</t>
   </si>
   <si>
-    <t xml:space="preserve">Overall_256_16</t>
+    <t xml:space="preserve">Overall_256</t>
   </si>
   <si>
     <t xml:space="preserve">Overall_256_8</t>
   </si>
   <si>
-    <t xml:space="preserve">Iteration_256_16</t>
+    <t xml:space="preserve">Iteration_256</t>
   </si>
   <si>
     <t xml:space="preserve">Iteration_256_8</t>
@@ -119,13 +119,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -150,6 +149,11 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -222,19 +226,19 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF5B9BD5"/>
       <rgbColor rgb="FF993366"/>
@@ -262,14 +266,14 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF70AD47"/>
       <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFED7D31"/>
       <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF70AD47"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -597,16 +601,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Overall_128_16</c:v>
+                  <c:v>Overall_128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Iteration_128_16</c:v>
+                  <c:v>Iteration_128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Overall_256_16</c:v>
+                  <c:v>Overall_256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Iteration_256_16</c:v>
+                  <c:v>Iteration_256</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -671,16 +675,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Overall_128_16</c:v>
+                  <c:v>Overall_128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Iteration_128_16</c:v>
+                  <c:v>Iteration_128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Overall_256_16</c:v>
+                  <c:v>Overall_256</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Iteration_256_16</c:v>
+                  <c:v>Iteration_256</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -709,11 +713,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="17743426"/>
-        <c:axId val="32774412"/>
+        <c:axId val="80155964"/>
+        <c:axId val="97466584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="17743426"/>
+        <c:axId val="80155964"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,14 +753,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32774412"/>
+        <c:crossAx val="97466584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32774412"/>
+        <c:axId val="97466584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +841,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17743426"/>
+        <c:crossAx val="80155964"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -849,16 +853,14 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.305477909011374"/>
-          <c:y val="0.907985564304462"/>
+          <c:x val="0.305420862862116"/>
+          <c:y val="0.907886104185802"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1027,11 +1029,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="95983623"/>
-        <c:axId val="92228922"/>
+        <c:axId val="77776253"/>
+        <c:axId val="94578220"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95983623"/>
+        <c:axId val="77776253"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,14 +1069,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92228922"/>
+        <c:crossAx val="94578220"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92228922"/>
+        <c:axId val="94578220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1117,7 +1119,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95983623"/>
+        <c:crossAx val="77776253"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1299,11 +1301,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="45023684"/>
-        <c:axId val="81403499"/>
+        <c:axId val="75738903"/>
+        <c:axId val="33213099"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="45023684"/>
+        <c:axId val="75738903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,14 +1341,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81403499"/>
+        <c:crossAx val="33213099"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81403499"/>
+        <c:axId val="33213099"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1391,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45023684"/>
+        <c:crossAx val="75738903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1424,20 +1426,225 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Collision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Boundaries</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Macroscopic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Residuals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>18.762087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.98168</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.355627</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.612173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.668854</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>285840</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>624960</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>590400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>210240</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1445,8 +1652,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15544800" y="114480"/>
-        <a:ext cx="5638320" cy="2742840"/>
+        <a:off x="17407800" y="3774240"/>
+        <a:ext cx="5681160" cy="2922120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1461,11 +1668,11 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>385920</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>80640</xdr:colOff>
+      <xdr:colOff>81360</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
@@ -1475,8 +1682,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15644880" y="3285720"/>
-        <a:ext cx="5790600" cy="2743200"/>
+        <a:off x="15644880" y="3287160"/>
+        <a:ext cx="5791320" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1495,9 +1702,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>114840</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1506,7 +1713,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2209680" y="4800600"/>
-        <a:ext cx="6333840" cy="2742840"/>
+        <a:ext cx="6334560" cy="2743560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1519,13 +1726,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>324000</xdr:colOff>
+      <xdr:colOff>325440</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>57240</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>333000</xdr:colOff>
+      <xdr:colOff>333720</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
@@ -1535,12 +1742,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8753400" y="4438440"/>
-        <a:ext cx="6076440" cy="2743200"/>
+        <a:off x="8754840" y="4439880"/>
+        <a:ext cx="6075720" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>519120</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>37080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4493880" y="797760"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1556,8 +1793,8 @@
   </sheetPr>
   <dimension ref="C1:J24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>